<commit_message>
ItemData에 Order 칼럼 추가
</commit_message>
<xml_diff>
--- a/excel/ItemData.xlsx
+++ b/excel/ItemData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F73715E-5C37-AA42-B634-F9A8759022BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EC5FAA-1E4B-1B43-9087-4F3FA08DCD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="5300" windowWidth="26220" windowHeight="11900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="5300" windowWidth="26220" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>string</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -382,6 +382,10 @@
   </si>
   <si>
     <t>Quantity</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -770,8 +774,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -794,6 +798,9 @@
       <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -808,6 +815,9 @@
       <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="7" t="s">
@@ -822,6 +832,9 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="7" t="s">
@@ -836,6 +849,9 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15">
       <c r="A5" s="7" t="s">
@@ -850,6 +866,9 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15">
       <c r="A6" s="7" t="s">
@@ -864,6 +883,9 @@
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15">
       <c r="A7" s="7" t="s">
@@ -878,6 +900,9 @@
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -891,6 +916,9 @@
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13">
@@ -906,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3404EB02-A5A0-8544-AC1C-24A6932127D0}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>